<commit_message>
fixed up the menu and added breath curves
</commit_message>
<xml_diff>
--- a/Documentation/EVI Main Timings.xlsx
+++ b/Documentation/EVI Main Timings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\Arduino\MidiEvi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\OneDrive\Documents\Arduino\MidiEvi\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2303B34C-A91F-4DDC-9226-5F18B059C53E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CEE562-A06C-4B89-BE18-5876262FDA06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="15390" windowHeight="9532" xr2:uid="{C43BFEC4-26F6-461B-B080-411462745667}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{C43BFEC4-26F6-461B-B080-411462745667}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -451,7 +451,7 @@
   <dimension ref="A1:J205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>